<commit_message>
TODO make lowtran /dev/null or NUL if can't open
</commit_message>
<xml_diff>
--- a/test/registration.xlsx
+++ b/test/registration.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,7 +33,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -102,10 +101,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -118,7 +115,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -132,10 +128,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -148,10 +142,8 @@
       <text>
         <r>
           <rPr>
-            <b val="true"/>
-            <sz val="8"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
+            <sz val="10"/>
+            <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
           </rPr>
@@ -167,7 +159,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -204,7 +195,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -219,7 +209,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -236,7 +225,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -250,7 +238,6 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
             <rFont val="Arial"/>
             <family val="2"/>
             <charset val="1"/>
@@ -321,19 +308,19 @@
     <t>BG3transFN</t>
   </si>
   <si>
-    <t>gridaurora/precompute/BG3transmittance.h5</t>
+    <t>../gridaurora/precompute/BG3transmittance.h5</t>
   </si>
   <si>
     <t>windowFN</t>
   </si>
   <si>
-    <t>gridaurora/precompute/ixonWindowT.h5</t>
+    <t>../gridaurora/precompute/ixonWindowT.h5</t>
   </si>
   <si>
     <t>emccdQEfn</t>
   </si>
   <si>
-    <t>gridaurora/precompute/emccdQE.h5</t>
+    <t>../gridaurora/precompute/emccdQE.h5</t>
   </si>
   <si>
     <t>TranscarDataDir</t>
@@ -378,7 +365,7 @@
     <t>reactionParam</t>
   </si>
   <si>
-    <t>gridaurora/precompute/vjeinfc.h5</t>
+    <t>../gridaurora/precompute/vjeinfc.h5</t>
   </si>
   <si>
     <t>altitudePreload</t>
@@ -1317,23 +1304,23 @@
   </sheetPr>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
+      <selection pane="bottomLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.9744897959184"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.1071428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.13775510204082"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.70408163265306"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.69897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="28.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.3469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.91836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.0816326530612"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="29.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2028,7 +2015,7 @@
   </sheetPr>
   <dimension ref="A1:IQ45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
@@ -2036,11 +2023,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="21.4030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="22.9744897959184"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="23.0459183673469"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="44" width="10.4132653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.4132653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="44" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="44" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9180,9 +9166,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3367346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4387755102041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.780612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7908163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.8775510204082"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>